<commit_message>
update BoM fix cek 08 mei 2020
</commit_message>
<xml_diff>
--- a/BOM_KrakatauBoardv1.3_Fix.xlsx
+++ b/BOM_KrakatauBoardv1.3_Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\projects\Krakatau Board v1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B71F2C85-893D-407D-BC02-77E044D005E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B644127-94D1-400B-BFC2-B25DF2BCD4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="345" windowWidth="28380" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="331">
   <si>
     <t>Item #</t>
   </si>
@@ -184,9 +183,6 @@
     <t xml:space="preserve">	Murata Electronics</t>
   </si>
   <si>
-    <t>BT1</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Harwin Inc.</t>
   </si>
   <si>
@@ -583,9 +579,6 @@
     <t>KEMET</t>
   </si>
   <si>
-    <t>C46</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/kemet/C0402C103M5RACTU/399-7760-1-ND/3471483</t>
   </si>
   <si>
@@ -646,9 +639,6 @@
     <t>FIXED IND 27NH 350MA 460 MOHM</t>
   </si>
   <si>
-    <t>C50</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/kemet/C0402C560K5RAC7867/399-C0402C560K5RAC7867CT-ND/11504529</t>
   </si>
   <si>
@@ -763,9 +753,6 @@
     <t>16-SOIC</t>
   </si>
   <si>
-    <t>BT2</t>
-  </si>
-  <si>
     <t>U13</t>
   </si>
   <si>
@@ -1042,12 +1029,6 @@
     <t xml:space="preserve">	CONN HEADER R/A 2POS 2.54MM</t>
   </si>
   <si>
-    <t>J3, J5, J11</t>
-  </si>
-  <si>
-    <t>J4, J6, J7</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/SWR25X-NRTC-S03-RB-BA/S9403-ND/2769661</t>
   </si>
   <si>
@@ -1076,6 +1057,36 @@
   </si>
   <si>
     <t>SMT MICRO SD CARD CONNECTOR, PUS</t>
+  </si>
+  <si>
+    <t>BT1, BT2</t>
+  </si>
+  <si>
+    <t>J3, J5, J11,  J13</t>
+  </si>
+  <si>
+    <t>J4, J6, J7, J14</t>
+  </si>
+  <si>
+    <t>C46, C50</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/61300511121/732-5318-ND/4846831</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 5POS 2.54MM</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 3POS 2.54MM	</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/61300311121/732-5316-ND/4846825</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1216,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1321,13 +1332,53 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1676,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1698,7 +1749,7 @@
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="D2" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="40"/>
@@ -1849,29 +1900,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="16" customFormat="1" ht="15">
@@ -1879,29 +1930,29 @@
         <v>5</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1915,29 +1966,29 @@
         <v>6</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -1951,7 +2002,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="8">
         <v>2</v>
@@ -1960,10 +2011,10 @@
         <v>28</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>26</v>
@@ -1973,7 +2024,7 @@
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -1987,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8">
         <v>2</v>
@@ -1996,10 +2047,10 @@
         <v>28</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>26</v>
@@ -2009,7 +2060,7 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="16" customFormat="1" ht="15">
@@ -2017,19 +2068,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="G15" s="8">
         <v>1210</v>
@@ -2039,7 +2090,7 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" ht="57">
@@ -2047,19 +2098,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C16" s="8">
         <v>21</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>26</v>
@@ -2069,7 +2120,7 @@
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="18" customFormat="1" ht="42.75">
@@ -2077,29 +2128,29 @@
         <v>11</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C17" s="8">
         <v>13</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="18" customFormat="1" ht="28.5">
@@ -2107,19 +2158,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C18" s="8">
         <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>26</v>
@@ -2129,7 +2180,7 @@
       </c>
       <c r="I18" s="22"/>
       <c r="J18" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2137,7 +2188,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
@@ -2146,20 +2197,20 @@
         <v>10</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2167,19 +2218,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C20" s="8">
         <v>3</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>26</v>
@@ -2189,7 +2240,7 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2197,29 +2248,29 @@
         <v>15</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="G21" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2227,29 +2278,29 @@
         <v>16</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="G22" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2257,19 +2308,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="24" t="s">
@@ -2277,7 +2328,7 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2285,7 +2336,7 @@
         <v>18</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
@@ -2294,20 +2345,20 @@
         <v>10</v>
       </c>
       <c r="E24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="24" t="s">
         <v>96</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>97</v>
       </c>
       <c r="H24" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2315,29 +2366,29 @@
         <v>19</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="8">
         <v>1</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="25">
         <v>865230542002</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H25" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2345,29 +2396,29 @@
         <v>20</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="G26" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2375,29 +2426,29 @@
         <v>21</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="G27" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2405,19 +2456,19 @@
         <v>22</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="8">
         <v>1</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>26</v>
@@ -2427,7 +2478,7 @@
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2435,19 +2486,19 @@
         <v>23</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" s="13">
         <v>78438356022</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="8" t="s">
@@ -2455,7 +2506,7 @@
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2463,29 +2514,29 @@
         <v>24</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H30" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I30" s="22"/>
       <c r="J30" s="11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2493,7 +2544,7 @@
         <v>25</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C31" s="28">
         <v>1</v>
@@ -2502,20 +2553,20 @@
         <v>10</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="G31" s="28" t="s">
         <v>119</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="H31" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2523,19 +2574,19 @@
         <v>26</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>26</v>
@@ -2545,7 +2596,7 @@
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2553,19 +2604,19 @@
         <v>27</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E33" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8" t="s">
@@ -2573,7 +2624,7 @@
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2581,19 +2632,19 @@
         <v>28</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="13">
         <v>5112</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>26</v>
@@ -2603,7 +2654,7 @@
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2611,7 +2662,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="8">
         <v>2</v>
@@ -2620,20 +2671,20 @@
         <v>10</v>
       </c>
       <c r="E35" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="G35" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2641,29 +2692,29 @@
         <v>30</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C36" s="8">
         <v>1</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="G36" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2671,29 +2722,29 @@
         <v>31</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E37" s="13">
         <v>742792651</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2701,19 +2752,19 @@
         <v>32</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="8">
         <v>2</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>26</v>
@@ -2723,7 +2774,7 @@
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2731,19 +2782,19 @@
         <v>33</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C39" s="8">
         <v>2</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E39" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>26</v>
@@ -2753,7 +2804,7 @@
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2761,19 +2812,19 @@
         <v>34</v>
       </c>
       <c r="B40" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="C40" s="24">
+        <v>2</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="24">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="F40" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>26</v>
@@ -2783,7 +2834,7 @@
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2791,19 +2842,19 @@
         <v>35</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E41" s="26">
         <v>885012105008</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>26</v>
@@ -2813,7 +2864,7 @@
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2821,29 +2872,29 @@
         <v>36</v>
       </c>
       <c r="B42" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="8">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="8">
-        <v>1</v>
-      </c>
-      <c r="D42" s="9" t="s">
+      <c r="E42" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2851,19 +2902,19 @@
         <v>37</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="8">
-        <v>1</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>176</v>
-      </c>
       <c r="F43" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="24" t="s">
@@ -2871,7 +2922,7 @@
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2879,19 +2930,19 @@
         <v>38</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C44" s="8">
-        <v>1</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>181</v>
-      </c>
       <c r="F44" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>26</v>
@@ -2901,27 +2952,27 @@
       </c>
       <c r="I44" s="10"/>
       <c r="J44" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A45" s="8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="8">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="C45" s="24">
-        <v>1</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>26</v>
@@ -2931,27 +2982,27 @@
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="11" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A46" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C46" s="8">
+        <v>2</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F46" s="13" t="s">
         <v>187</v>
-      </c>
-      <c r="C46" s="8">
-        <v>5</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>26</v>
@@ -2961,115 +3012,115 @@
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="11" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A47" s="8">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C47" s="8">
-        <v>2</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>188</v>
+        <v>1</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>192</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A48" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>195</v>
+      <c r="D48" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="G48" s="8"/>
+        <v>198</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>199</v>
+      </c>
       <c r="H48" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I48" s="10"/>
       <c r="J48" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A49" s="8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I49" s="10"/>
       <c r="J49" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A50" s="8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C50" s="8">
         <v>1</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>26</v>
@@ -3079,21 +3130,21 @@
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A51" s="8">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>208</v>
+        <v>296</v>
       </c>
       <c r="C51" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>210</v>
@@ -3101,9 +3152,7 @@
       <c r="F51" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="G51" s="8"/>
       <c r="H51" s="8" t="s">
         <v>9</v>
       </c>
@@ -3114,378 +3163,380 @@
     </row>
     <row r="52" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A52" s="8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>300</v>
+        <v>213</v>
       </c>
       <c r="C52" s="8">
-        <v>3</v>
-      </c>
-      <c r="D52" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E52" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8" t="s">
+      <c r="F52" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="H52" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I52" s="10"/>
       <c r="J52" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A53" s="8">
-        <v>47</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C53" s="8">
+        <v>49</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" s="28">
         <v>1</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="G53" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="H53" s="24" t="s">
+      <c r="F53" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H53" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="11" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A54" s="8">
-        <v>48</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="C54" s="8">
-        <v>1</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I54" s="21" t="s">
-        <v>62</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54" s="28">
+        <v>1</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G54" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H54" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" s="10"/>
       <c r="J54" s="11" t="s">
-        <v>33</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A55" s="8">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C55" s="28">
         <v>1</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="H55" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="G55" s="28">
+        <v>2818</v>
+      </c>
+      <c r="H55" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="11" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A56" s="8">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C56" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="G56" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="H56" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I56" s="10"/>
       <c r="J56" s="11" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A57" s="8">
-        <v>51</v>
-      </c>
-      <c r="B57" s="30" t="s">
-        <v>234</v>
+        <v>53</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>240</v>
       </c>
       <c r="C57" s="28">
         <v>1</v>
       </c>
-      <c r="D57" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="E57" s="29" t="s">
-        <v>236</v>
+      <c r="D57" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>242</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>237</v>
-      </c>
-      <c r="G57" s="28">
-        <v>2818</v>
-      </c>
-      <c r="H57" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="G57" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I57" s="10"/>
       <c r="J57" s="11" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A58" s="8">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C58" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="F58" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>26</v>
+        <v>249</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>66</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="11" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A59" s="8">
-        <v>53</v>
-      </c>
-      <c r="B59" s="27" t="s">
-        <v>244</v>
+        <v>55</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>260</v>
       </c>
       <c r="C59" s="28">
         <v>1</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>246</v>
+      <c r="D59" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>251</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="G59" s="31" t="s">
-        <v>249</v>
+        <v>252</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>253</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="11" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A60" s="8">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C60" s="28">
         <v>1</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="G60" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="H60" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="H60" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="11" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A61" s="8">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B61" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="28">
+        <v>1</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="C61" s="28">
-        <v>1</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>255</v>
-      </c>
       <c r="F61" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="G61" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="H61" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="G61" s="28"/>
+      <c r="H61" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="11" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A62" s="8">
-        <v>56</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>265</v>
+        <v>58</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>270</v>
       </c>
       <c r="C62" s="28">
         <v>1</v>
       </c>
-      <c r="D62" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="F62" s="29" t="s">
+      <c r="D62" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="G62" s="31" t="s">
+      <c r="F62" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="H62" s="31" t="s">
+      <c r="G62" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I62" s="10"/>
       <c r="J62" s="11" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A63" s="8">
-        <v>57</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>274</v>
       </c>
       <c r="C63" s="28">
-        <v>1</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="F63" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="G63" s="28"/>
-      <c r="H63" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I63" s="10"/>
       <c r="J63" s="11" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A64" s="8">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C64" s="28">
         <v>1</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>277</v>
+        <v>280</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>281</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>26</v>
@@ -3495,57 +3546,57 @@
       </c>
       <c r="I64" s="10"/>
       <c r="J64" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A65" s="8">
-        <v>59</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>278</v>
+        <v>61</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>282</v>
       </c>
       <c r="C65" s="28">
-        <v>2</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H65" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="G65" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="H65" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="11" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A66" s="8">
-        <v>60</v>
-      </c>
-      <c r="B66" s="27" t="s">
-        <v>282</v>
+        <v>62</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>287</v>
       </c>
       <c r="C66" s="28">
         <v>1</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>284</v>
+      <c r="D66" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>289</v>
       </c>
       <c r="F66" s="29" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>26</v>
@@ -3555,223 +3606,209 @@
       </c>
       <c r="I66" s="10"/>
       <c r="J66" s="11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="16" customFormat="1" ht="15">
-      <c r="A67" s="8">
-        <v>61</v>
-      </c>
-      <c r="B67" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="C67" s="28">
-        <v>1</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="E67" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="F67" s="29" t="s">
-        <v>289</v>
-      </c>
-      <c r="G67" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="H67" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I67" s="10"/>
-      <c r="J67" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" s="16" customFormat="1" ht="15">
-      <c r="A68" s="8">
-        <v>62</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="C68" s="28">
+    </row>
+    <row r="67" spans="1:10" ht="15">
+      <c r="A67" s="33"/>
+      <c r="B67" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C67" s="33">
+        <v>1</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="G67" s="33"/>
+      <c r="H67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67" s="35"/>
+      <c r="J67" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15">
+      <c r="A68" s="33"/>
+      <c r="B68" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="C68" s="33">
         <v>1</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E68" s="26">
+        <v>693071020811</v>
+      </c>
+      <c r="F68" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="G68" s="33"/>
       <c r="H68" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I68" s="10"/>
-      <c r="J68" s="11" t="s">
-        <v>292</v>
+      <c r="I68" s="35"/>
+      <c r="J68" s="4" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15">
       <c r="A69" s="33"/>
-      <c r="B69" s="37" t="s">
-        <v>307</v>
+      <c r="B69" s="34" t="s">
+        <v>297</v>
       </c>
       <c r="C69" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>304</v>
-      </c>
-      <c r="E69" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="F69" s="38" t="s">
-        <v>310</v>
+        <v>300</v>
+      </c>
+      <c r="E69" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F69" s="35" t="s">
+        <v>301</v>
       </c>
       <c r="G69" s="33"/>
-      <c r="H69" s="8" t="s">
-        <v>9</v>
+      <c r="H69" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="I69" s="35"/>
       <c r="J69" s="4" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15">
       <c r="A70" s="33"/>
       <c r="B70" s="37" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C70" s="33">
-        <v>1</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="26">
-        <v>693071020811</v>
+        <v>4</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>308</v>
       </c>
       <c r="F70" s="38" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="G70" s="33"/>
-      <c r="H70" s="8" t="s">
-        <v>9</v>
+      <c r="H70" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="I70" s="35"/>
       <c r="J70" s="4" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15">
       <c r="A71" s="33"/>
-      <c r="B71" s="34" t="s">
-        <v>301</v>
+      <c r="B71" s="37" t="s">
+        <v>323</v>
       </c>
       <c r="C71" s="33">
-        <v>2</v>
-      </c>
-      <c r="D71" s="35" t="s">
-        <v>304</v>
-      </c>
-      <c r="E71" s="35" t="s">
-        <v>303</v>
-      </c>
-      <c r="F71" s="35" t="s">
-        <v>305</v>
+        <v>4</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="F71" s="38" t="s">
+        <v>312</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="36" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I71" s="35"/>
       <c r="J71" s="4" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15">
       <c r="A72" s="33"/>
       <c r="B72" s="37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C72" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E72" s="38" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F72" s="38" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="G72" s="33"/>
       <c r="H72" s="36" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I72" s="35"/>
       <c r="J72" s="4" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15">
-      <c r="A73" s="33"/>
-      <c r="B73" s="37" t="s">
-        <v>316</v>
-      </c>
-      <c r="C73" s="33">
-        <v>3</v>
-      </c>
-      <c r="D73" s="38" t="s">
-        <v>313</v>
-      </c>
-      <c r="E73" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="F73" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="G73" s="33"/>
+      <c r="B73" s="42" t="s">
+        <v>325</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E73" s="43">
+        <v>61300511121</v>
+      </c>
+      <c r="F73" s="44" t="s">
+        <v>327</v>
+      </c>
       <c r="H73" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="I73" s="35"/>
+        <v>302</v>
+      </c>
       <c r="J73" s="4" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15">
-      <c r="A74" s="33"/>
-      <c r="B74" s="37" t="s">
-        <v>320</v>
-      </c>
-      <c r="C74" s="33">
-        <v>1</v>
-      </c>
-      <c r="D74" s="38" t="s">
-        <v>313</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="F74" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="G74" s="33"/>
+      <c r="B74" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E74" s="43">
+        <v>61300311121</v>
+      </c>
+      <c r="F74" s="44" t="s">
+        <v>329</v>
+      </c>
       <c r="H74" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="I74" s="35"/>
+        <v>302</v>
+      </c>
       <c r="J74" s="4" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3779,6 +3816,10 @@
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="J7" r:id="rId1" xr:uid="{45F037A1-B63B-4ED7-9A88-BEE8E6CBD7C5}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{CE384F57-86CE-4422-9E97-9FEE04A632FC}"/>
@@ -3816,38 +3857,38 @@
     <hyperlink ref="J41" r:id="rId34" xr:uid="{3E8EF905-2A64-4330-AA37-14EFAD895D9B}"/>
     <hyperlink ref="J42" r:id="rId35" xr:uid="{22918523-9B88-4A75-9B8C-D6CA7238D865}"/>
     <hyperlink ref="J44" r:id="rId36" xr:uid="{FA1E5006-1106-45F3-9BB0-D549D03DD9E2}"/>
-    <hyperlink ref="J45" r:id="rId37" xr:uid="{4A6C2BAD-2977-48DD-A3CB-2C1A4AB310AD}"/>
-    <hyperlink ref="J46" r:id="rId38" xr:uid="{F4B16AE1-8824-4085-93C1-8FB20244A2DD}"/>
-    <hyperlink ref="J47" r:id="rId39" xr:uid="{A9507617-23E8-4B06-81AF-D01F5DE904CB}"/>
-    <hyperlink ref="J48" r:id="rId40" xr:uid="{58B7C8C0-6517-4C98-8465-328DE873F14C}"/>
-    <hyperlink ref="J49" r:id="rId41" xr:uid="{0AE4E3F8-ED95-48E4-B59C-886F2F908C4A}"/>
-    <hyperlink ref="J50" r:id="rId42" xr:uid="{D41A5CF4-CE25-4943-B23E-5A5BC5975CAA}"/>
-    <hyperlink ref="J51" r:id="rId43" xr:uid="{E42E7D6E-D3E8-4BCF-A2EC-BD738F4F6C61}"/>
-    <hyperlink ref="J52" r:id="rId44" xr:uid="{94AB6D24-7DE4-42DC-9FC6-42BE8D63CAD7}"/>
-    <hyperlink ref="J53" r:id="rId45" xr:uid="{8EAB5F01-00FD-4C7E-B96F-9B74C632CD14}"/>
-    <hyperlink ref="J54" r:id="rId46" xr:uid="{DBB92050-ADE2-41A0-9C7B-144681174617}"/>
-    <hyperlink ref="J55" r:id="rId47" xr:uid="{1BF225B6-356B-41F6-B50D-EB1A0F4AFF63}"/>
-    <hyperlink ref="J56" r:id="rId48" xr:uid="{7EB2484F-C5A8-4998-A328-4C3F5E210473}"/>
-    <hyperlink ref="J57" r:id="rId49" xr:uid="{D57C496B-6F78-4BE1-BCA1-54D09C79A88E}"/>
-    <hyperlink ref="J58" r:id="rId50" xr:uid="{51DB1A6C-7E26-4B44-B703-758496F3117C}"/>
-    <hyperlink ref="J59" r:id="rId51" xr:uid="{C510970A-654C-44D2-8121-63B23819B46A}"/>
-    <hyperlink ref="J60" r:id="rId52" xr:uid="{5F8ABC6F-EF97-4899-A38A-6F9D533E9E0E}"/>
-    <hyperlink ref="J61" r:id="rId53" xr:uid="{14D2A9B2-FE59-4EF4-AE60-4B7FC5F9C83F}"/>
-    <hyperlink ref="J30" r:id="rId54" xr:uid="{10C2A7C9-9BA0-4DA7-A966-08D2DC785A1E}"/>
-    <hyperlink ref="J62" r:id="rId55" xr:uid="{702E9E8C-D694-4C5B-BD8D-340EC8E8C104}"/>
-    <hyperlink ref="J63" r:id="rId56" xr:uid="{E4926980-56B8-4342-8F3D-D29FE2CBF012}"/>
-    <hyperlink ref="J64" r:id="rId57" xr:uid="{909BFB48-DEF7-4C3F-A021-C9CD6F130515}"/>
-    <hyperlink ref="J65" r:id="rId58" xr:uid="{597A1AE5-DEAF-4DE9-80A6-9BA5EBEAF36E}"/>
-    <hyperlink ref="J66" r:id="rId59" xr:uid="{A93F37A2-6F1D-4AB7-924E-3058A184A0B1}"/>
-    <hyperlink ref="J67" r:id="rId60" xr:uid="{9184A80F-F197-4224-9256-4FFD541CEF82}"/>
-    <hyperlink ref="J68" r:id="rId61" xr:uid="{87BBCB41-78DF-4C5D-B5BB-D9FBFC752394}"/>
-    <hyperlink ref="J71" r:id="rId62" xr:uid="{F9ECDA17-7DE4-4CCC-B8F4-4A9E4A6C6F74}"/>
-    <hyperlink ref="J69" r:id="rId63" xr:uid="{D154315D-20A0-4824-AE06-DA7F6C9671A6}"/>
-    <hyperlink ref="J43" r:id="rId64" xr:uid="{E449F38B-B91A-4DD4-ABF6-22E7C202C751}"/>
-    <hyperlink ref="J72" r:id="rId65" xr:uid="{CBA38BF1-CE4B-4A83-AF5F-9A35D84C1A61}"/>
-    <hyperlink ref="J73" r:id="rId66" xr:uid="{701220A8-A80D-41C4-9831-B7FBC4DEAD13}"/>
-    <hyperlink ref="J74" r:id="rId67" xr:uid="{02EF8CF4-AEFB-45F0-AA07-4A61D0FEB7A8}"/>
-    <hyperlink ref="J70" r:id="rId68" xr:uid="{BEC2B2E0-269B-4E45-8CCD-E59B2140520C}"/>
+    <hyperlink ref="J45" r:id="rId37" xr:uid="{F4B16AE1-8824-4085-93C1-8FB20244A2DD}"/>
+    <hyperlink ref="J46" r:id="rId38" xr:uid="{A9507617-23E8-4B06-81AF-D01F5DE904CB}"/>
+    <hyperlink ref="J47" r:id="rId39" xr:uid="{58B7C8C0-6517-4C98-8465-328DE873F14C}"/>
+    <hyperlink ref="J48" r:id="rId40" xr:uid="{0AE4E3F8-ED95-48E4-B59C-886F2F908C4A}"/>
+    <hyperlink ref="J49" r:id="rId41" xr:uid="{D41A5CF4-CE25-4943-B23E-5A5BC5975CAA}"/>
+    <hyperlink ref="J50" r:id="rId42" xr:uid="{E42E7D6E-D3E8-4BCF-A2EC-BD738F4F6C61}"/>
+    <hyperlink ref="J51" r:id="rId43" xr:uid="{94AB6D24-7DE4-42DC-9FC6-42BE8D63CAD7}"/>
+    <hyperlink ref="J52" r:id="rId44" xr:uid="{8EAB5F01-00FD-4C7E-B96F-9B74C632CD14}"/>
+    <hyperlink ref="J53" r:id="rId45" xr:uid="{1BF225B6-356B-41F6-B50D-EB1A0F4AFF63}"/>
+    <hyperlink ref="J54" r:id="rId46" xr:uid="{7EB2484F-C5A8-4998-A328-4C3F5E210473}"/>
+    <hyperlink ref="J55" r:id="rId47" xr:uid="{D57C496B-6F78-4BE1-BCA1-54D09C79A88E}"/>
+    <hyperlink ref="J56" r:id="rId48" xr:uid="{51DB1A6C-7E26-4B44-B703-758496F3117C}"/>
+    <hyperlink ref="J57" r:id="rId49" xr:uid="{C510970A-654C-44D2-8121-63B23819B46A}"/>
+    <hyperlink ref="J58" r:id="rId50" xr:uid="{5F8ABC6F-EF97-4899-A38A-6F9D533E9E0E}"/>
+    <hyperlink ref="J59" r:id="rId51" xr:uid="{14D2A9B2-FE59-4EF4-AE60-4B7FC5F9C83F}"/>
+    <hyperlink ref="J30" r:id="rId52" xr:uid="{10C2A7C9-9BA0-4DA7-A966-08D2DC785A1E}"/>
+    <hyperlink ref="J60" r:id="rId53" xr:uid="{702E9E8C-D694-4C5B-BD8D-340EC8E8C104}"/>
+    <hyperlink ref="J61" r:id="rId54" xr:uid="{E4926980-56B8-4342-8F3D-D29FE2CBF012}"/>
+    <hyperlink ref="J62" r:id="rId55" xr:uid="{909BFB48-DEF7-4C3F-A021-C9CD6F130515}"/>
+    <hyperlink ref="J63" r:id="rId56" xr:uid="{597A1AE5-DEAF-4DE9-80A6-9BA5EBEAF36E}"/>
+    <hyperlink ref="J64" r:id="rId57" xr:uid="{A93F37A2-6F1D-4AB7-924E-3058A184A0B1}"/>
+    <hyperlink ref="J65" r:id="rId58" xr:uid="{9184A80F-F197-4224-9256-4FFD541CEF82}"/>
+    <hyperlink ref="J66" r:id="rId59" xr:uid="{87BBCB41-78DF-4C5D-B5BB-D9FBFC752394}"/>
+    <hyperlink ref="J69" r:id="rId60" xr:uid="{F9ECDA17-7DE4-4CCC-B8F4-4A9E4A6C6F74}"/>
+    <hyperlink ref="J67" r:id="rId61" xr:uid="{D154315D-20A0-4824-AE06-DA7F6C9671A6}"/>
+    <hyperlink ref="J43" r:id="rId62" xr:uid="{E449F38B-B91A-4DD4-ABF6-22E7C202C751}"/>
+    <hyperlink ref="J70" r:id="rId63" xr:uid="{CBA38BF1-CE4B-4A83-AF5F-9A35D84C1A61}"/>
+    <hyperlink ref="J71" r:id="rId64" xr:uid="{701220A8-A80D-41C4-9831-B7FBC4DEAD13}"/>
+    <hyperlink ref="J72" r:id="rId65" xr:uid="{02EF8CF4-AEFB-45F0-AA07-4A61D0FEB7A8}"/>
+    <hyperlink ref="J68" r:id="rId66" xr:uid="{BEC2B2E0-269B-4E45-8CCD-E59B2140520C}"/>
+    <hyperlink ref="J73" r:id="rId67" xr:uid="{EB44634B-9E26-47F3-956D-51AE301ABA09}"/>
+    <hyperlink ref="J74" r:id="rId68" xr:uid="{28D0D3FC-4A80-4780-BDBF-1F1C46D0256F}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId69"/>

</xml_diff>

<commit_message>
vias 0.25 min pcbway for 2mm
</commit_message>
<xml_diff>
--- a/BOM_KrakatauBoardv1.3_Fix.xlsx
+++ b/BOM_KrakatauBoardv1.3_Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\projects\Krakatau Board v1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B644127-94D1-400B-BFC2-B25DF2BCD4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD947292-C2D6-4D03-AC13-666E7AFCEA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="345" windowWidth="28380" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="329">
   <si>
     <t>Item #</t>
   </si>
@@ -348,21 +356,9 @@
     <t>CAP CER 4.7UF 16V X7R 0805</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics/LQH32PH2R2NNCL/490-16006-1-ND/6800671</t>
-  </si>
-  <si>
-    <t>LQH32PH2R2NNCL</t>
-  </si>
-  <si>
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t xml:space="preserve">FIXED IND 2.2UH 1.85A 76.8 MOHM	</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/vishay-dale/TNPW040210K0BETD/541-3559-1-ND/7354920</t>
   </si>
   <si>
@@ -402,9 +398,6 @@
     <t xml:space="preserve">CAP CER 0.22UF 50V X7R 0805	</t>
   </si>
   <si>
-    <t>C29, C30</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/taiyo-yuden/LMK212BBJ226MD-T/587-5917-1-ND/7675037</t>
   </si>
   <si>
@@ -462,9 +455,6 @@
     <t>CAP CER 0.47UF 10V X7R 0402</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/78438356022/732-11314-1-ND/6833773</t>
   </si>
   <si>
@@ -1087,6 +1077,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/w%C3%BCrth-elektronik/61300311121/732-5316-ND/4846825</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>C29, C30, C63, C64</t>
+  </si>
+  <si>
+    <t>smd</t>
+  </si>
+  <si>
+    <t>th</t>
   </si>
 </sst>
 </file>
@@ -1324,6 +1326,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1332,32 +1343,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1725,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:P74"/>
+  <dimension ref="A2:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="E30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1746,25 +1738,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="19.5" customHeight="1">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="D2" s="39" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="D2" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="6" spans="1:16" ht="28.5" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1900,7 +1892,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
@@ -2098,7 +2090,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C16" s="8">
         <v>21</v>
@@ -2128,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C17" s="8">
         <v>13</v>
@@ -2158,7 +2150,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C18" s="8">
         <v>7</v>
@@ -2167,10 +2159,10 @@
         <v>73</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>26</v>
@@ -2180,7 +2172,7 @@
       </c>
       <c r="I18" s="22"/>
       <c r="J18" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2218,7 +2210,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C20" s="8">
         <v>3</v>
@@ -2307,58 +2299,60 @@
       <c r="A23" s="8">
         <v>17</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>84</v>
+      <c r="B23" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="23"/>
+        <v>91</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>92</v>
+      </c>
       <c r="H23" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A24" s="8">
         <v>18</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>92</v>
+      <c r="B24" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>94</v>
+        <v>122</v>
+      </c>
+      <c r="E24" s="25">
+        <v>865230542002</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>96</v>
+        <v>121</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="H24" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="11" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2366,29 +2360,29 @@
         <v>19</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="8">
-        <v>1</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="25">
-        <v>865230542002</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25" s="24" t="s">
+      <c r="G25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="11" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2396,19 +2390,19 @@
         <v>20</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>98</v>
+        <v>326</v>
       </c>
       <c r="C26" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="E26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>60</v>
@@ -2418,37 +2412,37 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A27" s="8">
         <v>21</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>102</v>
+      <c r="B27" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" s="9" t="s">
+      <c r="E27" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G27" s="23" t="s">
-        <v>60</v>
+      <c r="F27" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2456,117 +2450,117 @@
         <v>22</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>108</v>
+        <v>325</v>
       </c>
       <c r="C28" s="8">
-        <v>1</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>110</v>
+        <v>2</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="13">
+        <v>78438356022</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G28" s="7"/>
       <c r="H28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="11" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A29" s="8">
         <v>23</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>122</v>
+      <c r="B29" s="20" t="s">
+        <v>285</v>
       </c>
       <c r="C29" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" s="13">
-        <v>78438356022</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="10"/>
+        <v>250</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="22"/>
       <c r="J29" s="11" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A30" s="8">
         <v>24</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="C30" s="8">
+      <c r="B30" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="28">
         <v>1</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="22"/>
+        <v>10</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="10"/>
       <c r="J30" s="11" t="s">
-        <v>255</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A31" s="8">
         <v>25</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="28">
-        <v>1</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" s="28" t="s">
+      <c r="F31" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2574,29 +2568,27 @@
         <v>26</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>26</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G32" s="8"/>
       <c r="H32" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2604,57 +2596,59 @@
         <v>27</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="8"/>
+      <c r="E33" s="13">
+        <v>5112</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H33" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A34" s="8">
         <v>28</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="8">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="13">
-        <v>5112</v>
-      </c>
       <c r="F34" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2662,13 +2656,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>140</v>
@@ -2684,7 +2678,7 @@
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2698,16 +2692,16 @@
         <v>1</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="13">
+        <v>742792651</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="G36" s="7" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>9</v>
@@ -2722,29 +2716,29 @@
         <v>31</v>
       </c>
       <c r="B37" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="8">
+        <v>2</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="13">
-        <v>742792651</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="G37" s="7" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2752,19 +2746,19 @@
         <v>32</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38" s="8">
         <v>2</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>26</v>
@@ -2774,7 +2768,7 @@
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2782,19 +2776,19 @@
         <v>33</v>
       </c>
       <c r="B39" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="C39" s="24">
+        <v>2</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C39" s="8">
-        <v>2</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="F39" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>26</v>
@@ -2804,7 +2798,7 @@
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2812,19 +2806,19 @@
         <v>34</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C40" s="24">
-        <v>2</v>
+        <v>158</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="26">
+        <v>885012105008</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>26</v>
@@ -2834,7 +2828,7 @@
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2842,59 +2836,57 @@
         <v>35</v>
       </c>
       <c r="B41" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="8">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="8">
-        <v>1</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E41" s="26">
-        <v>885012105008</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H41" s="8" t="s">
+      <c r="G41" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H41" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A42" s="8">
         <v>36</v>
       </c>
-      <c r="B42" s="20" t="s">
-        <v>167</v>
+      <c r="B42" s="12" t="s">
+        <v>166</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>169</v>
+      <c r="D42" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>171</v>
-      </c>
+      <c r="F42" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42" s="8"/>
       <c r="H42" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I42" s="10"/>
-      <c r="J42" s="11" t="s">
-        <v>173</v>
+      <c r="J42" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2902,27 +2894,29 @@
         <v>37</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="10"/>
+      <c r="J43" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="C43" s="8">
-        <v>1</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="16" customFormat="1" ht="15">
@@ -2930,19 +2924,19 @@
         <v>38</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="8">
+        <v>5</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="C44" s="8">
-        <v>1</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>180</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>26</v>
@@ -2952,27 +2946,27 @@
       </c>
       <c r="I44" s="10"/>
       <c r="J44" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A45" s="8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C45" s="8">
-        <v>5</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>160</v>
+        <v>2</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>26</v>
@@ -2982,70 +2976,70 @@
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A46" s="8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="C46" s="8">
-        <v>2</v>
-      </c>
-      <c r="D46" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A47" s="8">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="F47" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E47" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F47" s="13" t="s">
+      <c r="G47" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A48" s="8">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>194</v>
@@ -3054,16 +3048,16 @@
         <v>1</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>197</v>
+        <v>28</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>196</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>9</v>
@@ -3075,22 +3069,22 @@
     </row>
     <row r="49" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A49" s="8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="E49" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>202</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>203</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>26</v>
@@ -3100,90 +3094,90 @@
       </c>
       <c r="I49" s="10"/>
       <c r="J49" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A50" s="8">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="C50" s="8">
+        <v>3</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="C50" s="8">
-        <v>1</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="G50" s="8"/>
       <c r="H50" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A51" s="8">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>296</v>
+        <v>207</v>
       </c>
       <c r="C51" s="8">
-        <v>3</v>
-      </c>
-      <c r="D51" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G51" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A52" s="8">
-        <v>47</v>
-      </c>
-      <c r="B52" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="28">
         <v>1</v>
       </c>
       <c r="D52" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G52" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="H52" s="24" t="s">
+      <c r="G52" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H52" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I52" s="10"/>
@@ -3193,37 +3187,37 @@
     </row>
     <row r="53" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A53" s="8">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C53" s="28">
         <v>1</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>221</v>
       </c>
       <c r="F53" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="G53" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A54" s="8">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B54" s="30" t="s">
         <v>224</v>
@@ -3232,16 +3226,16 @@
         <v>1</v>
       </c>
       <c r="D54" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E54" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="E54" s="29" t="s">
+      <c r="F54" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="F54" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="G54" s="31" t="s">
-        <v>229</v>
+      <c r="G54" s="28">
+        <v>2818</v>
       </c>
       <c r="H54" s="31" t="s">
         <v>9</v>
@@ -3253,85 +3247,85 @@
     </row>
     <row r="55" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A55" s="8">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C55" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F55" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="G55" s="28">
-        <v>2818</v>
-      </c>
-      <c r="H55" s="31" t="s">
+      <c r="G55" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A56" s="8">
-        <v>52</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>235</v>
+        <v>50</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>234</v>
       </c>
       <c r="C56" s="28">
-        <v>2</v>
-      </c>
-      <c r="D56" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F56" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="E56" s="29" t="s">
-        <v>237</v>
-      </c>
-      <c r="F56" s="29" t="s">
+      <c r="G56" s="31" t="s">
         <v>239</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I56" s="10"/>
       <c r="J56" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A57" s="8">
-        <v>53</v>
-      </c>
-      <c r="B57" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="30" t="s">
         <v>240</v>
       </c>
       <c r="C57" s="28">
         <v>1</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="F57" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E57" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="F57" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>245</v>
+      <c r="G57" s="32" t="s">
+        <v>66</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>9</v>
@@ -3343,140 +3337,140 @@
     </row>
     <row r="58" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A58" s="8">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B58" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="C58" s="28">
+        <v>1</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="F58" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="C58" s="28">
-        <v>1</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="G58" s="32" t="s">
-        <v>66</v>
+      <c r="G58" s="28" t="s">
+        <v>247</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A59" s="8">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B59" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="C59" s="28">
+        <v>1</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="E59" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C59" s="28">
-        <v>1</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>254</v>
-      </c>
-      <c r="E59" s="29" t="s">
-        <v>251</v>
-      </c>
       <c r="F59" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="H59" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="H59" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="11" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A60" s="8">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>261</v>
+        <v>11</v>
       </c>
       <c r="C60" s="28">
         <v>1</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>267</v>
+        <v>191</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="G60" s="31" t="s">
-        <v>269</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="G60" s="28"/>
       <c r="H60" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="11" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A61" s="8">
-        <v>57</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>264</v>
       </c>
       <c r="C61" s="28">
         <v>1</v>
       </c>
-      <c r="D61" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="F61" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="G61" s="28"/>
-      <c r="H61" s="31" t="s">
+      <c r="D61" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A62" s="8">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B62" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C62" s="28">
+        <v>2</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C62" s="28">
-        <v>1</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="F62" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>26</v>
@@ -3486,27 +3480,27 @@
       </c>
       <c r="I62" s="10"/>
       <c r="J62" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A63" s="8">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B63" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" s="28">
+        <v>1</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E63" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C63" s="28">
-        <v>2</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>277</v>
+      <c r="F63" s="29" t="s">
+        <v>275</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>26</v>
@@ -3516,115 +3510,115 @@
       </c>
       <c r="I63" s="10"/>
       <c r="J63" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A64" s="8">
-        <v>60</v>
-      </c>
-      <c r="B64" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="28">
+        <v>1</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E64" s="29" t="s">
         <v>278</v>
       </c>
-      <c r="C64" s="28">
-        <v>1</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E64" s="10" t="s">
+      <c r="F64" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="G64" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="F64" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="G64" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H64" s="8" t="s">
+      <c r="H64" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I64" s="10"/>
       <c r="J64" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="16" customFormat="1" ht="15">
       <c r="A65" s="8">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C65" s="28">
         <v>1</v>
       </c>
-      <c r="D65" s="29" t="s">
-        <v>176</v>
+      <c r="D65" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="E65" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="F65" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="F65" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="G65" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="H65" s="31" t="s">
+      <c r="G65" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="16" customFormat="1" ht="15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15">
       <c r="A66" s="8">
-        <v>62</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>287</v>
-      </c>
-      <c r="C66" s="28">
-        <v>1</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>289</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C66" s="33">
+        <v>1</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="F66" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="G66" s="33"/>
       <c r="H66" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I66" s="10"/>
-      <c r="J66" s="11" t="s">
-        <v>288</v>
+      <c r="I66" s="35"/>
+      <c r="J66" s="4" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15">
-      <c r="A67" s="33"/>
+      <c r="A67" s="8">
+        <v>61</v>
+      </c>
       <c r="B67" s="37" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="C67" s="33">
         <v>1</v>
       </c>
-      <c r="D67" s="35" t="s">
-        <v>300</v>
-      </c>
-      <c r="E67" s="38" t="s">
-        <v>305</v>
+      <c r="D67" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E67" s="26">
+        <v>693071020811</v>
       </c>
       <c r="F67" s="38" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="G67" s="33"/>
       <c r="H67" s="8" t="s">
@@ -3632,183 +3626,193 @@
       </c>
       <c r="I67" s="35"/>
       <c r="J67" s="4" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15">
-      <c r="A68" s="33"/>
-      <c r="B68" s="37" t="s">
-        <v>319</v>
+      <c r="A68" s="8">
+        <v>62</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="C68" s="33">
-        <v>1</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E68" s="26">
-        <v>693071020811</v>
-      </c>
-      <c r="F68" s="38" t="s">
-        <v>320</v>
+        <v>2</v>
+      </c>
+      <c r="D68" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="E68" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="F68" s="35" t="s">
+        <v>295</v>
       </c>
       <c r="G68" s="33"/>
-      <c r="H68" s="8" t="s">
-        <v>9</v>
+      <c r="H68" s="36" t="s">
+        <v>296</v>
       </c>
       <c r="I68" s="35"/>
       <c r="J68" s="4" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15">
-      <c r="A69" s="33"/>
-      <c r="B69" s="34" t="s">
-        <v>297</v>
+      <c r="A69" s="8">
+        <v>63</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>316</v>
       </c>
       <c r="C69" s="33">
-        <v>2</v>
-      </c>
-      <c r="D69" s="35" t="s">
-        <v>300</v>
-      </c>
-      <c r="E69" s="35" t="s">
-        <v>299</v>
-      </c>
-      <c r="F69" s="35" t="s">
-        <v>301</v>
+        <v>4</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="F69" s="38" t="s">
+        <v>304</v>
       </c>
       <c r="G69" s="33"/>
       <c r="H69" s="36" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="I69" s="35"/>
       <c r="J69" s="4" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15">
-      <c r="A70" s="33"/>
+      <c r="A70" s="8">
+        <v>64</v>
+      </c>
       <c r="B70" s="37" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C70" s="33">
         <v>4</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E70" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F70" s="38" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G70" s="33"/>
       <c r="H70" s="36" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="I70" s="35"/>
       <c r="J70" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15">
-      <c r="A71" s="33"/>
+      <c r="A71" s="8">
+        <v>65</v>
+      </c>
       <c r="B71" s="37" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C71" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D71" s="38" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E71" s="38" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F71" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="36" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="I71" s="35"/>
       <c r="J71" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15">
-      <c r="A72" s="33"/>
-      <c r="B72" s="37" t="s">
-        <v>314</v>
-      </c>
-      <c r="C72" s="33">
-        <v>1</v>
-      </c>
-      <c r="D72" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="E72" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="F72" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="G72" s="33"/>
+      <c r="A72" s="8">
+        <v>66</v>
+      </c>
+      <c r="B72" s="39" t="s">
+        <v>319</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" s="40">
+        <v>61300511121</v>
+      </c>
+      <c r="F72" s="41" t="s">
+        <v>321</v>
+      </c>
       <c r="H72" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="I72" s="35"/>
+        <v>296</v>
+      </c>
       <c r="J72" s="4" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15">
-      <c r="B73" s="42" t="s">
-        <v>325</v>
+      <c r="A73" s="8">
+        <v>67</v>
+      </c>
+      <c r="B73" s="39" t="s">
+        <v>322</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E73" s="43">
-        <v>61300511121</v>
-      </c>
-      <c r="F73" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="40">
+        <v>61300311121</v>
+      </c>
+      <c r="F73" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="D76" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="H73" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="15">
-      <c r="B74" s="42" t="s">
+      <c r="E76" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" s="43">
-        <v>61300311121</v>
-      </c>
-      <c r="F74" s="44" t="s">
-        <v>329</v>
-      </c>
-      <c r="H74" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>330</v>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="C77" s="1">
+        <f>SUM(C7:C73)</f>
+        <v>136</v>
+      </c>
+      <c r="D77" s="2">
+        <f>SUM(C7:C67)</f>
+        <v>123</v>
+      </c>
+      <c r="E77" s="2">
+        <f>SUM(C68:C73)</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3817,8 +3821,8 @@
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="J7" r:id="rId1" xr:uid="{45F037A1-B63B-4ED7-9A88-BEE8E6CBD7C5}"/>
@@ -3836,63 +3840,62 @@
     <hyperlink ref="J20" r:id="rId13" xr:uid="{B1ADCB0D-071E-4DA9-A238-55942F48ED10}"/>
     <hyperlink ref="J22" r:id="rId14" xr:uid="{CD32033A-E9A9-4605-BE09-6853ABCA0764}"/>
     <hyperlink ref="J21" r:id="rId15" xr:uid="{1770C22D-D978-4F0A-A0DF-719DF98544D8}"/>
-    <hyperlink ref="J23" r:id="rId16" xr:uid="{5DD1A015-030A-4C2E-9092-E99AA0A59EF4}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{FA382E1B-E2FB-49BD-97BD-81359F1DD750}"/>
-    <hyperlink ref="J24" r:id="rId18" xr:uid="{E02206FE-FECC-4DDA-99F2-CBCC0F9DF9C4}"/>
-    <hyperlink ref="J26" r:id="rId19" xr:uid="{F6903F40-01C0-46D0-8E79-2E4D135579A3}"/>
-    <hyperlink ref="J27" r:id="rId20" xr:uid="{4EA02204-3DF6-4463-8414-2339FEBF9B7B}"/>
-    <hyperlink ref="J28" r:id="rId21" xr:uid="{6F6EBC93-C08F-48E1-B272-0A08C3427452}"/>
-    <hyperlink ref="J32" r:id="rId22" xr:uid="{6717480D-EDE7-4E4A-AB9B-0E3BB5A5E9D2}"/>
-    <hyperlink ref="J31" r:id="rId23" xr:uid="{9DD14C6B-E3BB-4F6F-A488-0B239B5D3296}"/>
-    <hyperlink ref="J29" r:id="rId24" xr:uid="{55F68D89-CFD7-49AC-9D95-9FA43514D858}"/>
-    <hyperlink ref="J25" r:id="rId25" xr:uid="{7ADAA259-7FE2-4D79-80AB-44FA59EA60AF}"/>
-    <hyperlink ref="J33" r:id="rId26" xr:uid="{607B774F-F20B-45CA-B896-7D75DD879486}"/>
-    <hyperlink ref="J34" r:id="rId27" xr:uid="{353E1094-19E6-477E-BC00-0DA0FB427AF0}"/>
-    <hyperlink ref="J35" r:id="rId28" xr:uid="{6866481B-471D-45FA-B439-0737954AE6B4}"/>
-    <hyperlink ref="J36" r:id="rId29" xr:uid="{9D06B25D-6C5B-4B32-99B8-9B1A98DC83FB}"/>
-    <hyperlink ref="J37" r:id="rId30" xr:uid="{DE7C64A0-6A22-411E-BAB2-04B4184B7DC2}"/>
-    <hyperlink ref="J38" r:id="rId31" xr:uid="{2F51FE19-93BE-44C3-B58A-A7F565FDDB77}"/>
-    <hyperlink ref="J39" r:id="rId32" xr:uid="{C7DA621E-4EA0-4CA4-BA1B-31890EE3D8EC}"/>
-    <hyperlink ref="J40" r:id="rId33" xr:uid="{D1C1E11A-EF18-456E-9E84-ACB8644FA178}"/>
-    <hyperlink ref="J41" r:id="rId34" xr:uid="{3E8EF905-2A64-4330-AA37-14EFAD895D9B}"/>
-    <hyperlink ref="J42" r:id="rId35" xr:uid="{22918523-9B88-4A75-9B8C-D6CA7238D865}"/>
-    <hyperlink ref="J44" r:id="rId36" xr:uid="{FA1E5006-1106-45F3-9BB0-D549D03DD9E2}"/>
-    <hyperlink ref="J45" r:id="rId37" xr:uid="{F4B16AE1-8824-4085-93C1-8FB20244A2DD}"/>
-    <hyperlink ref="J46" r:id="rId38" xr:uid="{A9507617-23E8-4B06-81AF-D01F5DE904CB}"/>
-    <hyperlink ref="J47" r:id="rId39" xr:uid="{58B7C8C0-6517-4C98-8465-328DE873F14C}"/>
-    <hyperlink ref="J48" r:id="rId40" xr:uid="{0AE4E3F8-ED95-48E4-B59C-886F2F908C4A}"/>
-    <hyperlink ref="J49" r:id="rId41" xr:uid="{D41A5CF4-CE25-4943-B23E-5A5BC5975CAA}"/>
-    <hyperlink ref="J50" r:id="rId42" xr:uid="{E42E7D6E-D3E8-4BCF-A2EC-BD738F4F6C61}"/>
-    <hyperlink ref="J51" r:id="rId43" xr:uid="{94AB6D24-7DE4-42DC-9FC6-42BE8D63CAD7}"/>
-    <hyperlink ref="J52" r:id="rId44" xr:uid="{8EAB5F01-00FD-4C7E-B96F-9B74C632CD14}"/>
-    <hyperlink ref="J53" r:id="rId45" xr:uid="{1BF225B6-356B-41F6-B50D-EB1A0F4AFF63}"/>
-    <hyperlink ref="J54" r:id="rId46" xr:uid="{7EB2484F-C5A8-4998-A328-4C3F5E210473}"/>
-    <hyperlink ref="J55" r:id="rId47" xr:uid="{D57C496B-6F78-4BE1-BCA1-54D09C79A88E}"/>
-    <hyperlink ref="J56" r:id="rId48" xr:uid="{51DB1A6C-7E26-4B44-B703-758496F3117C}"/>
-    <hyperlink ref="J57" r:id="rId49" xr:uid="{C510970A-654C-44D2-8121-63B23819B46A}"/>
-    <hyperlink ref="J58" r:id="rId50" xr:uid="{5F8ABC6F-EF97-4899-A38A-6F9D533E9E0E}"/>
-    <hyperlink ref="J59" r:id="rId51" xr:uid="{14D2A9B2-FE59-4EF4-AE60-4B7FC5F9C83F}"/>
-    <hyperlink ref="J30" r:id="rId52" xr:uid="{10C2A7C9-9BA0-4DA7-A966-08D2DC785A1E}"/>
-    <hyperlink ref="J60" r:id="rId53" xr:uid="{702E9E8C-D694-4C5B-BD8D-340EC8E8C104}"/>
-    <hyperlink ref="J61" r:id="rId54" xr:uid="{E4926980-56B8-4342-8F3D-D29FE2CBF012}"/>
-    <hyperlink ref="J62" r:id="rId55" xr:uid="{909BFB48-DEF7-4C3F-A021-C9CD6F130515}"/>
-    <hyperlink ref="J63" r:id="rId56" xr:uid="{597A1AE5-DEAF-4DE9-80A6-9BA5EBEAF36E}"/>
-    <hyperlink ref="J64" r:id="rId57" xr:uid="{A93F37A2-6F1D-4AB7-924E-3058A184A0B1}"/>
-    <hyperlink ref="J65" r:id="rId58" xr:uid="{9184A80F-F197-4224-9256-4FFD541CEF82}"/>
-    <hyperlink ref="J66" r:id="rId59" xr:uid="{87BBCB41-78DF-4C5D-B5BB-D9FBFC752394}"/>
-    <hyperlink ref="J69" r:id="rId60" xr:uid="{F9ECDA17-7DE4-4CCC-B8F4-4A9E4A6C6F74}"/>
-    <hyperlink ref="J67" r:id="rId61" xr:uid="{D154315D-20A0-4824-AE06-DA7F6C9671A6}"/>
-    <hyperlink ref="J43" r:id="rId62" xr:uid="{E449F38B-B91A-4DD4-ABF6-22E7C202C751}"/>
-    <hyperlink ref="J70" r:id="rId63" xr:uid="{CBA38BF1-CE4B-4A83-AF5F-9A35D84C1A61}"/>
-    <hyperlink ref="J71" r:id="rId64" xr:uid="{701220A8-A80D-41C4-9831-B7FBC4DEAD13}"/>
-    <hyperlink ref="J72" r:id="rId65" xr:uid="{02EF8CF4-AEFB-45F0-AA07-4A61D0FEB7A8}"/>
-    <hyperlink ref="J68" r:id="rId66" xr:uid="{BEC2B2E0-269B-4E45-8CCD-E59B2140520C}"/>
-    <hyperlink ref="J73" r:id="rId67" xr:uid="{EB44634B-9E26-47F3-956D-51AE301ABA09}"/>
-    <hyperlink ref="J74" r:id="rId68" xr:uid="{28D0D3FC-4A80-4780-BDBF-1F1C46D0256F}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{FA382E1B-E2FB-49BD-97BD-81359F1DD750}"/>
+    <hyperlink ref="J23" r:id="rId17" xr:uid="{E02206FE-FECC-4DDA-99F2-CBCC0F9DF9C4}"/>
+    <hyperlink ref="J25" r:id="rId18" xr:uid="{F6903F40-01C0-46D0-8E79-2E4D135579A3}"/>
+    <hyperlink ref="J26" r:id="rId19" xr:uid="{4EA02204-3DF6-4463-8414-2339FEBF9B7B}"/>
+    <hyperlink ref="J27" r:id="rId20" xr:uid="{6F6EBC93-C08F-48E1-B272-0A08C3427452}"/>
+    <hyperlink ref="J31" r:id="rId21" xr:uid="{6717480D-EDE7-4E4A-AB9B-0E3BB5A5E9D2}"/>
+    <hyperlink ref="J30" r:id="rId22" xr:uid="{9DD14C6B-E3BB-4F6F-A488-0B239B5D3296}"/>
+    <hyperlink ref="J28" r:id="rId23" xr:uid="{55F68D89-CFD7-49AC-9D95-9FA43514D858}"/>
+    <hyperlink ref="J24" r:id="rId24" xr:uid="{7ADAA259-7FE2-4D79-80AB-44FA59EA60AF}"/>
+    <hyperlink ref="J32" r:id="rId25" xr:uid="{607B774F-F20B-45CA-B896-7D75DD879486}"/>
+    <hyperlink ref="J33" r:id="rId26" xr:uid="{353E1094-19E6-477E-BC00-0DA0FB427AF0}"/>
+    <hyperlink ref="J34" r:id="rId27" xr:uid="{6866481B-471D-45FA-B439-0737954AE6B4}"/>
+    <hyperlink ref="J35" r:id="rId28" xr:uid="{9D06B25D-6C5B-4B32-99B8-9B1A98DC83FB}"/>
+    <hyperlink ref="J36" r:id="rId29" xr:uid="{DE7C64A0-6A22-411E-BAB2-04B4184B7DC2}"/>
+    <hyperlink ref="J37" r:id="rId30" xr:uid="{2F51FE19-93BE-44C3-B58A-A7F565FDDB77}"/>
+    <hyperlink ref="J38" r:id="rId31" xr:uid="{C7DA621E-4EA0-4CA4-BA1B-31890EE3D8EC}"/>
+    <hyperlink ref="J39" r:id="rId32" xr:uid="{D1C1E11A-EF18-456E-9E84-ACB8644FA178}"/>
+    <hyperlink ref="J40" r:id="rId33" xr:uid="{3E8EF905-2A64-4330-AA37-14EFAD895D9B}"/>
+    <hyperlink ref="J41" r:id="rId34" xr:uid="{22918523-9B88-4A75-9B8C-D6CA7238D865}"/>
+    <hyperlink ref="J43" r:id="rId35" xr:uid="{FA1E5006-1106-45F3-9BB0-D549D03DD9E2}"/>
+    <hyperlink ref="J44" r:id="rId36" xr:uid="{F4B16AE1-8824-4085-93C1-8FB20244A2DD}"/>
+    <hyperlink ref="J45" r:id="rId37" xr:uid="{A9507617-23E8-4B06-81AF-D01F5DE904CB}"/>
+    <hyperlink ref="J46" r:id="rId38" xr:uid="{58B7C8C0-6517-4C98-8465-328DE873F14C}"/>
+    <hyperlink ref="J47" r:id="rId39" xr:uid="{0AE4E3F8-ED95-48E4-B59C-886F2F908C4A}"/>
+    <hyperlink ref="J48" r:id="rId40" xr:uid="{D41A5CF4-CE25-4943-B23E-5A5BC5975CAA}"/>
+    <hyperlink ref="J49" r:id="rId41" xr:uid="{E42E7D6E-D3E8-4BCF-A2EC-BD738F4F6C61}"/>
+    <hyperlink ref="J50" r:id="rId42" xr:uid="{94AB6D24-7DE4-42DC-9FC6-42BE8D63CAD7}"/>
+    <hyperlink ref="J51" r:id="rId43" xr:uid="{8EAB5F01-00FD-4C7E-B96F-9B74C632CD14}"/>
+    <hyperlink ref="J52" r:id="rId44" xr:uid="{1BF225B6-356B-41F6-B50D-EB1A0F4AFF63}"/>
+    <hyperlink ref="J53" r:id="rId45" xr:uid="{7EB2484F-C5A8-4998-A328-4C3F5E210473}"/>
+    <hyperlink ref="J54" r:id="rId46" xr:uid="{D57C496B-6F78-4BE1-BCA1-54D09C79A88E}"/>
+    <hyperlink ref="J55" r:id="rId47" xr:uid="{51DB1A6C-7E26-4B44-B703-758496F3117C}"/>
+    <hyperlink ref="J56" r:id="rId48" xr:uid="{C510970A-654C-44D2-8121-63B23819B46A}"/>
+    <hyperlink ref="J57" r:id="rId49" xr:uid="{5F8ABC6F-EF97-4899-A38A-6F9D533E9E0E}"/>
+    <hyperlink ref="J58" r:id="rId50" xr:uid="{14D2A9B2-FE59-4EF4-AE60-4B7FC5F9C83F}"/>
+    <hyperlink ref="J29" r:id="rId51" xr:uid="{10C2A7C9-9BA0-4DA7-A966-08D2DC785A1E}"/>
+    <hyperlink ref="J59" r:id="rId52" xr:uid="{702E9E8C-D694-4C5B-BD8D-340EC8E8C104}"/>
+    <hyperlink ref="J60" r:id="rId53" xr:uid="{E4926980-56B8-4342-8F3D-D29FE2CBF012}"/>
+    <hyperlink ref="J61" r:id="rId54" xr:uid="{909BFB48-DEF7-4C3F-A021-C9CD6F130515}"/>
+    <hyperlink ref="J62" r:id="rId55" xr:uid="{597A1AE5-DEAF-4DE9-80A6-9BA5EBEAF36E}"/>
+    <hyperlink ref="J63" r:id="rId56" xr:uid="{A93F37A2-6F1D-4AB7-924E-3058A184A0B1}"/>
+    <hyperlink ref="J64" r:id="rId57" xr:uid="{9184A80F-F197-4224-9256-4FFD541CEF82}"/>
+    <hyperlink ref="J65" r:id="rId58" xr:uid="{87BBCB41-78DF-4C5D-B5BB-D9FBFC752394}"/>
+    <hyperlink ref="J68" r:id="rId59" xr:uid="{F9ECDA17-7DE4-4CCC-B8F4-4A9E4A6C6F74}"/>
+    <hyperlink ref="J66" r:id="rId60" xr:uid="{D154315D-20A0-4824-AE06-DA7F6C9671A6}"/>
+    <hyperlink ref="J42" r:id="rId61" xr:uid="{E449F38B-B91A-4DD4-ABF6-22E7C202C751}"/>
+    <hyperlink ref="J69" r:id="rId62" xr:uid="{CBA38BF1-CE4B-4A83-AF5F-9A35D84C1A61}"/>
+    <hyperlink ref="J70" r:id="rId63" xr:uid="{701220A8-A80D-41C4-9831-B7FBC4DEAD13}"/>
+    <hyperlink ref="J71" r:id="rId64" xr:uid="{02EF8CF4-AEFB-45F0-AA07-4A61D0FEB7A8}"/>
+    <hyperlink ref="J67" r:id="rId65" xr:uid="{BEC2B2E0-269B-4E45-8CCD-E59B2140520C}"/>
+    <hyperlink ref="J72" r:id="rId66" xr:uid="{EB44634B-9E26-47F3-956D-51AE301ABA09}"/>
+    <hyperlink ref="J73" r:id="rId67" xr:uid="{28D0D3FC-4A80-4780-BDBF-1F1C46D0256F}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId69"/>
-  <drawing r:id="rId70"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId68"/>
+  <drawing r:id="rId69"/>
 </worksheet>
 </file>
 

</xml_diff>